<commit_message>
Excel Sheet output update
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/RegistrationData.xlsx
+++ b/src/test/resources/TestData/RegistrationData.xlsx
@@ -3,20 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vigne\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14350" windowHeight="3490"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="69">
   <si>
     <t>FirstName</t>
   </si>
@@ -210,12 +207,43 @@
   </si>
   <si>
     <t>Review UI accessibility.</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Registeration Success</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for presence of element located by: By.xpath: //p[text()='Let us know how we can help you! '] (tried for 10 second(s) with 500 milliseconds interval)</t>
+  </si>
+  <si>
+    <t>invalid session id: session deleted as the browser has closed the connection
+from disconnected: not connected to DevTools
+  (Session info: chrome=138.0.7204.51)
+Build info: version: '4.34.0', revision: '707dcb4246*'
+System info: os.name: 'Windows 11', os.arch: 'amd64', os.version: '10.0', java.version: '17.0.10'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Command: [16afb3713cfc2db653323f8892db7681, getElementText {id=f.29C03CE9A8A12171843F1D5CBECF27D8.d.EFC12B82C93D294CF895C5FF8B0969E4.e.78}]
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 138.0.7204.51, chrome: {chromedriverVersion: 138.0.7204.92 (f079b9bc781e..., userDataDir: C:\Users\vigne\AppData\Loca...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:64649}, networkConnectionEnabled: false, pageLoadStrategy: normal, platformName: windows, proxy: Proxy(), se:cdp: ws://localhost:64649/devtoo..., se:cdpVersion: 138.0.7204.51, setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Element: [[ChromeDriver: chrome on windows (16afb3713cfc2db653323f8892db7681)] -&gt; xpath: //p[text()='Let us know how we can help you! ']]
+Session ID: 16afb3713cfc2db653323f8892db7681</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -541,24 +569,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" customWidth="1"/>
-    <col min="3" max="3" width="36.08984375" customWidth="1"/>
-    <col min="4" max="4" width="15.90625" customWidth="1"/>
-    <col min="5" max="5" width="18.90625" customWidth="1"/>
-    <col min="6" max="6" width="23.54296875" customWidth="1"/>
-    <col min="7" max="7" width="38.7265625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="12.1796875"/>
+    <col min="2" max="2" customWidth="true" width="15.453125"/>
+    <col min="3" max="3" customWidth="true" width="36.08984375"/>
+    <col min="4" max="4" customWidth="true" width="15.90625"/>
+    <col min="5" max="5" customWidth="true" width="18.90625"/>
+    <col min="6" max="6" customWidth="true" width="23.54296875"/>
+    <col min="7" max="7" customWidth="true" width="38.7265625"/>
+    <col min="9" max="9" customWidth="true" width="28.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -580,8 +609,14 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -603,8 +638,14 @@
       <c r="G2" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -626,8 +667,14 @@
       <c r="G3" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H3" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -649,8 +696,14 @@
       <c r="G4" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -672,147 +725,168 @@
       <c r="G5" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1122334455</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="2">
-        <v>5566778899</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="2">
-        <v>3344556677</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="2">
-        <v>2233445566</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" s="2">
-        <v>6677889900</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" s="2">
-        <v>7788990011</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>61</v>
+      <c r="H5" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="2">
+        <v>1122334455</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="2">
+        <v>5566778899</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3344556677</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2233445566</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="2">
+        <v>6677889900</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="2">
+        <v>7788990011</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>